<commit_message>
finish fst hw 2022-01-21
</commit_message>
<xml_diff>
--- a/小数点 - 用户画像/第一周文件合集/第一周作业/作业问题1&3.xlsx
+++ b/小数点 - 用户画像/第一周文件合集/第一周作业/作业问题1&3.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13420"/>
+    <workbookView windowWidth="28800" windowHeight="13400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="83">
   <si>
     <t>问题1：</t>
   </si>
@@ -239,6 +240,30 @@
   </si>
   <si>
     <t>点赞次数</t>
+  </si>
+  <si>
+    <t>问题3：</t>
+  </si>
+  <si>
+    <t>模拟面试场景，准备 1 分钟介绍用户画像的内容（200个字左右）。</t>
+  </si>
+  <si>
+    <t>回答：</t>
+  </si>
+  <si>
+    <t>我理解中的用户画像，是公司为了更好地识别出用户的特征，从抽象到具体，建立的一套可以全方位管理用户特征的数据系统。</t>
+  </si>
+  <si>
+    <t>抽象，指的是公司服务的用户特性，比如，星巴克的用户画像，抽象起来就是喜欢和咖啡的较高收入的群体。</t>
+  </si>
+  <si>
+    <t>而具体表现在，使用一个360度的标签体系描述每一个来到公司的用户特征，并记录用户全生命周期的特征。</t>
+  </si>
+  <si>
+    <t>用户画像是可以贯穿公司业务形态的系统，它可以服务于前端前台，也可以在中台和后台发挥作用。</t>
+  </si>
+  <si>
+    <t>通过用户画像系统，就能在不同的业务，比如精准营销，识别风险，CRM客户管理等等，更好地识别目标群体，降低公司成本，最大化地提高活动收益。</t>
   </si>
 </sst>
 </file>
@@ -246,13 +271,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -268,21 +301,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -294,6 +312,38 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -305,6 +355,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -314,17 +386,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -336,9 +408,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -346,29 +417,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,9 +431,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -396,29 +444,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -429,90 +454,114 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -525,7 +574,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,79 +610,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,9 +733,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -719,32 +746,15 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -780,6 +790,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -794,162 +828,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -963,7 +988,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
@@ -1301,11 +1326,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="B3:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
@@ -1317,23 +1342,23 @@
   </cols>
   <sheetData>
     <row r="3" ht="20.4" spans="2:3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" ht="20.4" spans="2:3">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="2"/>
+      <c r="B5" s="1"/>
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -1344,24 +1369,24 @@
       </c>
     </row>
     <row r="7" ht="20.4" spans="2:3">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="2"/>
+      <c r="B8" s="1"/>
       <c r="C8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" ht="20.4" spans="2:3">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1946,4 +1971,59 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="1"/>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3">
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3">
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>